<commit_message>
updated data names to underscore format
</commit_message>
<xml_diff>
--- a/nda/pessiglione_data_definition.xlsx
+++ b/nda/pessiglione_data_definition.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pessiglionne\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pessiglionne\nda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A43F8ACF-05A7-4478-9F2F-A528A0BCBA19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB34FF1-E948-4609-9EB9-5DA81E74F931}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="34005" windowHeight="20265" xr2:uid="{F703BFBF-BC98-4E10-835D-060D0FF4CAF5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="96">
   <si>
     <t>ElementName</t>
   </si>
@@ -173,9 +173,6 @@
     <t>valid,invalid</t>
   </si>
   <si>
-    <t>pairTrialsPerBlock</t>
-  </si>
-  <si>
     <t>how many times in a block is this stimulus pair presented</t>
   </si>
   <si>
@@ -315,6 +312,15 @@
   </si>
   <si>
     <t>0:1</t>
+  </si>
+  <si>
+    <t>pair_trials_per_block</t>
+  </si>
+  <si>
+    <t>participant_response</t>
+  </si>
+  <si>
+    <t>participant response, same as key_press</t>
   </si>
 </sst>
 </file>
@@ -669,14 +675,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7C1E109-CA05-4F93-BB2E-D7A1E92CF0A6}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="104.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -874,81 +882,81 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
         <v>47</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>48</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
         <v>50</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>51</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
       </c>
       <c r="D15" t="s">
         <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
         <v>59</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
       </c>
       <c r="D17" t="s">
         <v>34</v>
@@ -956,13 +964,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
         <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>62</v>
       </c>
       <c r="D18" t="s">
         <v>34</v>
@@ -970,38 +978,38 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
         <v>63</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
         <v>65</v>
       </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
-      </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
         <v>67</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
@@ -1009,13 +1017,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
         <v>69</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" t="s">
-        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>34</v>
@@ -1023,89 +1031,89 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
         <v>71</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>72</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>73</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>15</v>
       </c>
       <c r="C24" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" t="s">
         <v>76</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>77</v>
-      </c>
-      <c r="E24" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
         <v>34</v>
       </c>
       <c r="E26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
         <v>15</v>
       </c>
       <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
         <v>85</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" t="s">
         <v>15</v>
@@ -1122,36 +1130,53 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
       </c>
       <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D29" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
         <v>15</v>
       </c>
       <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>91</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="D30" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>